<commit_message>
Quadratic growth in nr images to be expected.
</commit_message>
<xml_diff>
--- a/gtsam_unstable/base/tests/timeDSFvariants.xlsx
+++ b/gtsam_unstable/base/tests/timeDSFvariants.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27540" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dsf-timing.csv" sheetId="1" r:id="rId1"/>
@@ -430,11 +430,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2137971480"/>
-        <c:axId val="2137968312"/>
+        <c:axId val="2139027672"/>
+        <c:axId val="2138715288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2137971480"/>
+        <c:axId val="2139027672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -444,12 +444,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137968312"/>
+        <c:crossAx val="2138715288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2137968312"/>
+        <c:axId val="2138715288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -461,7 +461,370 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137971480"/>
+        <c:crossAx val="2139027672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'dsf-timing.csv'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Base</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'dsf-timing.csv'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'dsf-timing.csv'!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>6.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000497</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001358</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.001866</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01063</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.034276</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.080089</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.120456</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.172458</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'dsf-timing.csv'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'dsf-timing.csv'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'dsf-timing.csv'!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.000909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.003468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.010806</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.034243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.054209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.319107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.17656</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.98121</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.93586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'dsf-timing.csv'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BTree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'dsf-timing.csv'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'dsf-timing.csv'!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.032572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.091209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.279008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.575306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.937282</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7954</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.3224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.9018</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.4166</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>118.404</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2102908632"/>
+        <c:axId val="2135719816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2102908632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2135719816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2135719816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2102908632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -488,19 +851,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -510,6 +873,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -843,7 +1236,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>